<commit_message>
numbering change May 28th
</commit_message>
<xml_diff>
--- a/06_pagevolume/동아리 관리 앱 제작.xlsx
+++ b/06_pagevolume/동아리 관리 앱 제작.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Do\Desktop\동아리 관리 어플 제작\project_file\06_pagevolume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC73BF2-BCBD-44DC-8F1E-A43E4919D009}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7060B831-ED10-400C-8A89-2EF963221DD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{D03F7F62-3720-4364-8511-30CBD7CEB86D}"/>
   </bookViews>
@@ -446,10 +446,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13. 투표</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>문자 받는 이 검색</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -853,6 +849,10 @@
   </si>
   <si>
     <t xml:space="preserve"> Target Club in DongA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12. 투표</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1256,89 +1256,89 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0BACC9-CED0-4164-BABB-29AF74952461}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79:J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1679,18 +1679,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36" customHeight="1">
-      <c r="A1" s="64" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="A1" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="22.5">
       <c r="A2" s="21" t="s">
@@ -1712,7 +1712,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>5</v>
@@ -1728,23 +1728,23 @@
       <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="23">
         <v>2</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="63" t="s">
         <v>70</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1757,7 +1757,7 @@
         <v>20</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I4" s="12" t="s">
         <v>77</v>
@@ -1770,7 +1770,7 @@
       <c r="A5" s="23">
         <v>3</v>
       </c>
-      <c r="B5" s="37"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="11" t="s">
         <v>72</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>12</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="25">
@@ -1792,7 +1792,7 @@
       <c r="A6" s="23">
         <v>4</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
         <v>74</v>
@@ -1801,7 +1801,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="25">
@@ -1812,7 +1812,7 @@
       <c r="A7" s="23">
         <v>5</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="11" t="s">
         <v>73</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="25">
@@ -1834,7 +1834,7 @@
       <c r="A8" s="23">
         <v>6</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="13"/>
       <c r="D8" s="9" t="s">
         <v>75</v>
@@ -1843,7 +1843,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>78</v>
@@ -1856,7 +1856,7 @@
       <c r="A9" s="23">
         <v>7</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="13"/>
       <c r="D9" s="9" t="s">
         <v>79</v>
@@ -1865,7 +1865,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="25">
@@ -1876,23 +1876,23 @@
       <c r="A10" s="23">
         <v>8</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="23">
         <v>9</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="46" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="14"/>
@@ -1910,7 +1910,7 @@
       <c r="A12" s="23">
         <v>10</v>
       </c>
-      <c r="B12" s="46"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="11" t="s">
         <v>80</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>12</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="25">
@@ -1932,7 +1932,7 @@
       <c r="A13" s="23">
         <v>11</v>
       </c>
-      <c r="B13" s="46"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="15"/>
       <c r="D13" s="9" t="s">
         <v>82</v>
@@ -1941,7 +1941,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="25">
@@ -1952,7 +1952,7 @@
       <c r="A14" s="23">
         <v>12</v>
       </c>
-      <c r="B14" s="46"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
         <v>83</v>
@@ -1963,7 +1963,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="25">
@@ -1974,23 +1974,23 @@
       <c r="A15" s="23">
         <v>13</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1">
       <c r="A16" s="23">
         <v>14</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="26"/>
@@ -2008,7 +2008,7 @@
       <c r="A17" s="23">
         <v>15</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
@@ -2030,7 +2030,7 @@
       <c r="A18" s="23">
         <v>16</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
         <v>22</v>
@@ -2050,7 +2050,7 @@
       <c r="A19" s="23">
         <v>17</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="A20" s="23">
         <v>18</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
@@ -2094,7 +2094,7 @@
       <c r="A21" s="23">
         <v>19</v>
       </c>
-      <c r="B21" s="41"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="5" t="s">
         <v>19</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>21</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>67</v>
@@ -2118,23 +2118,23 @@
       <c r="A22" s="23">
         <v>20</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="23">
         <v>21</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="40" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -2160,7 +2160,7 @@
       <c r="A24" s="23">
         <v>22</v>
       </c>
-      <c r="B24" s="41"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9" t="s">
         <v>13</v>
@@ -2184,7 +2184,7 @@
       <c r="A25" s="23">
         <v>23</v>
       </c>
-      <c r="B25" s="41"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="5" t="s">
         <v>19</v>
       </c>
@@ -2208,7 +2208,7 @@
       <c r="A26" s="23">
         <v>24</v>
       </c>
-      <c r="B26" s="41"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="5" t="s">
         <v>8</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="A27" s="23">
         <v>25</v>
       </c>
-      <c r="B27" s="41"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
         <v>30</v>
@@ -2256,7 +2256,7 @@
       <c r="A28" s="23">
         <v>26</v>
       </c>
-      <c r="B28" s="41"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
@@ -2280,24 +2280,24 @@
       <c r="A29" s="23">
         <v>27</v>
       </c>
-      <c r="B29" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
+      <c r="B29" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="23">
         <v>28</v>
       </c>
-      <c r="B30" s="46" t="s">
-        <v>130</v>
+      <c r="B30" s="47" t="s">
+        <v>129</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>89</v>
@@ -2309,7 +2309,7 @@
         <v>12</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I30" s="28"/>
       <c r="J30" s="25">
@@ -2320,7 +2320,7 @@
       <c r="A31" s="23">
         <v>29</v>
       </c>
-      <c r="B31" s="46"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
         <v>93</v>
@@ -2329,7 +2329,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I31" s="29"/>
       <c r="J31" s="25">
@@ -2340,7 +2340,7 @@
       <c r="A32" s="23">
         <v>30</v>
       </c>
-      <c r="B32" s="46"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="11" t="s">
         <v>90</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>12</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I32" s="28"/>
       <c r="J32" s="24">
@@ -2362,7 +2362,7 @@
       <c r="A33" s="23">
         <v>31</v>
       </c>
-      <c r="B33" s="46"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="13"/>
       <c r="D33" s="9" t="s">
         <v>91</v>
@@ -2373,7 +2373,7 @@
         <v>20</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I33" s="29"/>
       <c r="J33" s="24"/>
@@ -2382,7 +2382,7 @@
       <c r="A34" s="23">
         <v>32</v>
       </c>
-      <c r="B34" s="46"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="13"/>
       <c r="D34" s="9" t="s">
         <v>92</v>
@@ -2393,7 +2393,7 @@
         <v>21</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I34" s="29"/>
       <c r="J34" s="25">
@@ -2404,7 +2404,7 @@
       <c r="A35" s="23">
         <v>33</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="16"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8" t="s">
@@ -2413,7 +2413,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I35" s="30"/>
       <c r="J35" s="25"/>
@@ -2422,7 +2422,7 @@
       <c r="A36" s="23">
         <v>34</v>
       </c>
-      <c r="B36" s="53"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="11" t="s">
         <v>94</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>12</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I36" s="28"/>
       <c r="J36" s="25"/>
@@ -2442,23 +2442,23 @@
       <c r="A37" s="23">
         <v>35</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="23">
         <v>36</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="61" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -2482,7 +2482,7 @@
       <c r="A39" s="23">
         <v>37</v>
       </c>
-      <c r="B39" s="41"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="5" t="s">
         <v>19</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="A40" s="23">
         <v>38</v>
       </c>
-      <c r="B40" s="41"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="5" t="s">
         <v>8</v>
       </c>
@@ -2517,10 +2517,10 @@
         <v>11</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J40" s="24">
         <v>2</v>
@@ -2530,27 +2530,27 @@
       <c r="A41" s="23">
         <v>39</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="56"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="51"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="23">
         <v>40</v>
       </c>
-      <c r="B42" s="49" t="s">
-        <v>108</v>
+      <c r="B42" s="41" t="s">
+        <v>107</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -2559,10 +2559,10 @@
         <v>20</v>
       </c>
       <c r="H42" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J42" s="24">
         <v>4</v>
@@ -2573,9 +2573,9 @@
       <c r="A43" s="23">
         <v>41</v>
       </c>
-      <c r="B43" s="50"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -2584,10 +2584,10 @@
         <v>12</v>
       </c>
       <c r="H43" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="I43" s="57" t="s">
-        <v>184</v>
+        <v>157</v>
+      </c>
+      <c r="I43" s="52" t="s">
+        <v>183</v>
       </c>
       <c r="J43" s="24">
         <v>5</v>
@@ -2598,18 +2598,18 @@
       <c r="A44" s="23">
         <v>42</v>
       </c>
-      <c r="B44" s="50"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="I44" s="58"/>
+        <v>133</v>
+      </c>
+      <c r="I44" s="53"/>
       <c r="J44" s="24">
         <v>5</v>
       </c>
@@ -2619,18 +2619,18 @@
       <c r="A45" s="23">
         <v>43</v>
       </c>
-      <c r="B45" s="50"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="I45" s="59"/>
+        <v>134</v>
+      </c>
+      <c r="I45" s="54"/>
       <c r="J45" s="24">
         <v>5</v>
       </c>
@@ -2640,9 +2640,9 @@
       <c r="A46" s="23">
         <v>44</v>
       </c>
-      <c r="B46" s="51"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -2651,7 +2651,7 @@
         <v>12</v>
       </c>
       <c r="H46" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I46" s="31"/>
       <c r="J46" s="24">
@@ -2663,27 +2663,27 @@
       <c r="A47" s="23">
         <v>45</v>
       </c>
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="56"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="51"/>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="23">
         <v>46</v>
       </c>
-      <c r="B48" s="60" t="s">
-        <v>185</v>
+      <c r="B48" s="55" t="s">
+        <v>184</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -2692,7 +2692,7 @@
         <v>12</v>
       </c>
       <c r="H48" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I48" s="28"/>
       <c r="J48" s="24">
@@ -2704,16 +2704,16 @@
       <c r="A49" s="23">
         <v>47</v>
       </c>
-      <c r="B49" s="50"/>
+      <c r="B49" s="42"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I49" s="29"/>
       <c r="J49" s="24">
@@ -2725,9 +2725,9 @@
       <c r="A50" s="23">
         <v>48</v>
       </c>
-      <c r="B50" s="50"/>
+      <c r="B50" s="42"/>
       <c r="C50" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -2736,7 +2736,7 @@
         <v>12</v>
       </c>
       <c r="H50" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I50" s="28"/>
       <c r="J50" s="24">
@@ -2748,7 +2748,7 @@
       <c r="A51" s="23">
         <v>49</v>
       </c>
-      <c r="B51" s="50"/>
+      <c r="B51" s="42"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9" t="s">
         <v>79</v>
@@ -2757,7 +2757,7 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I51" s="29"/>
       <c r="J51" s="24">
@@ -2769,7 +2769,7 @@
       <c r="A52" s="23">
         <v>50</v>
       </c>
-      <c r="B52" s="51"/>
+      <c r="B52" s="43"/>
       <c r="C52" s="5" t="s">
         <v>94</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>12</v>
       </c>
       <c r="H52" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I52" s="28"/>
       <c r="J52" s="24">
@@ -2792,27 +2792,27 @@
       <c r="A53" s="23">
         <v>51</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
-      <c r="H53" s="55"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="56"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="51"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="23">
         <v>52</v>
       </c>
-      <c r="B54" s="49" t="s">
+      <c r="B54" s="41" t="s">
         <v>86</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
@@ -2821,10 +2821,10 @@
         <v>12</v>
       </c>
       <c r="H54" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="I54" s="61" t="s">
-        <v>117</v>
+        <v>136</v>
+      </c>
+      <c r="I54" s="56" t="s">
+        <v>116</v>
       </c>
       <c r="J54" s="24">
         <v>5</v>
@@ -2835,9 +2835,9 @@
       <c r="A55" s="23">
         <v>53</v>
       </c>
-      <c r="B55" s="50"/>
+      <c r="B55" s="42"/>
       <c r="C55" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -2846,9 +2846,9 @@
         <v>12</v>
       </c>
       <c r="H55" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="I55" s="62"/>
+        <v>162</v>
+      </c>
+      <c r="I55" s="57"/>
       <c r="J55" s="24">
         <v>5</v>
       </c>
@@ -2858,9 +2858,9 @@
       <c r="A56" s="23">
         <v>54</v>
       </c>
-      <c r="B56" s="50"/>
+      <c r="B56" s="42"/>
       <c r="C56" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -2869,9 +2869,9 @@
         <v>12</v>
       </c>
       <c r="H56" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="I56" s="63"/>
+        <v>163</v>
+      </c>
+      <c r="I56" s="58"/>
       <c r="J56" s="24">
         <v>5</v>
       </c>
@@ -2881,9 +2881,9 @@
       <c r="A57" s="23">
         <v>55</v>
       </c>
-      <c r="B57" s="50"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -2892,7 +2892,7 @@
         <v>12</v>
       </c>
       <c r="H57" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I57" s="32"/>
       <c r="J57" s="25">
@@ -2904,7 +2904,7 @@
       <c r="A58" s="23">
         <v>56</v>
       </c>
-      <c r="B58" s="50"/>
+      <c r="B58" s="42"/>
       <c r="C58" s="5" t="s">
         <v>87</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>12</v>
       </c>
       <c r="H58" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I58" s="32"/>
       <c r="J58" s="25">
@@ -2927,19 +2927,19 @@
       <c r="A59" s="23">
         <v>57</v>
       </c>
-      <c r="B59" s="50"/>
+      <c r="B59" s="42"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I59" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J59" s="25">
         <v>1</v>
@@ -2950,18 +2950,18 @@
       <c r="A60" s="23">
         <v>58</v>
       </c>
-      <c r="B60" s="51"/>
+      <c r="B60" s="43"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I60" s="30"/>
       <c r="J60" s="25">
@@ -2973,23 +2973,23 @@
       <c r="A61" s="23">
         <v>59</v>
       </c>
-      <c r="B61" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
+      <c r="B61" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="23">
         <v>60</v>
       </c>
-      <c r="B62" s="45" t="s">
+      <c r="B62" s="46" t="s">
         <v>53</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -3015,7 +3015,7 @@
       <c r="A63" s="23">
         <v>61</v>
       </c>
-      <c r="B63" s="46"/>
+      <c r="B63" s="47"/>
       <c r="C63" s="11" t="s">
         <v>55</v>
       </c>
@@ -3026,10 +3026,10 @@
         <v>56</v>
       </c>
       <c r="H63" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J63" s="25">
         <v>1</v>
@@ -3039,10 +3039,10 @@
       <c r="A64" s="23">
         <v>62</v>
       </c>
-      <c r="B64" s="46"/>
+      <c r="B64" s="47"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
@@ -3050,10 +3050,10 @@
         <v>63</v>
       </c>
       <c r="H64" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I64" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J64" s="25">
         <v>1</v>
@@ -3063,10 +3063,10 @@
       <c r="A65" s="23">
         <v>63</v>
       </c>
-      <c r="B65" s="46"/>
+      <c r="B65" s="47"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
@@ -3074,10 +3074,10 @@
         <v>64</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I65" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J65" s="25">
         <v>1</v>
@@ -3087,7 +3087,7 @@
       <c r="A66" s="23">
         <v>64</v>
       </c>
-      <c r="B66" s="46"/>
+      <c r="B66" s="47"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9" t="s">
         <v>60</v>
@@ -3098,10 +3098,10 @@
         <v>56</v>
       </c>
       <c r="H66" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I66" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J66" s="25">
         <v>1</v>
@@ -3111,7 +3111,7 @@
       <c r="A67" s="23">
         <v>65</v>
       </c>
-      <c r="B67" s="46"/>
+      <c r="B67" s="47"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9" t="s">
         <v>61</v>
@@ -3122,10 +3122,10 @@
         <v>41</v>
       </c>
       <c r="H67" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I67" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J67" s="25">
         <v>2</v>
@@ -3135,19 +3135,19 @@
       <c r="A68" s="23">
         <v>66</v>
       </c>
-      <c r="B68" s="46"/>
+      <c r="B68" s="47"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="33"/>
       <c r="H68" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="I68" s="29" t="s">
         <v>201</v>
-      </c>
-      <c r="I68" s="29" t="s">
-        <v>202</v>
       </c>
       <c r="J68" s="25">
         <v>2</v>
@@ -3157,7 +3157,7 @@
       <c r="A69" s="23">
         <v>67</v>
       </c>
-      <c r="B69" s="46"/>
+      <c r="B69" s="47"/>
       <c r="C69" s="13"/>
       <c r="D69" s="9" t="s">
         <v>62</v>
@@ -3168,10 +3168,10 @@
         <v>12</v>
       </c>
       <c r="H69" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J69" s="25">
         <v>2</v>
@@ -3181,7 +3181,7 @@
       <c r="A70" s="23">
         <v>68</v>
       </c>
-      <c r="B70" s="46"/>
+      <c r="B70" s="47"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9" t="s">
         <v>65</v>
@@ -3192,7 +3192,7 @@
         <v>68</v>
       </c>
       <c r="H70" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I70" s="29"/>
       <c r="J70" s="25">
@@ -3203,7 +3203,7 @@
       <c r="A71" s="23">
         <v>69</v>
       </c>
-      <c r="B71" s="53"/>
+      <c r="B71" s="48"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9" t="s">
         <v>69</v>
@@ -3214,7 +3214,7 @@
         <v>66</v>
       </c>
       <c r="H71" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I71" s="29" t="s">
         <v>67</v>
@@ -3227,23 +3227,23 @@
       <c r="A72" s="23">
         <v>70</v>
       </c>
-      <c r="B72" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="C72" s="42"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="42"/>
-      <c r="F72" s="42"/>
-      <c r="G72" s="42"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="42"/>
-      <c r="J72" s="42"/>
+      <c r="B72" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="44"/>
+      <c r="J72" s="44"/>
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="23">
         <v>71</v>
       </c>
-      <c r="B73" s="37" t="s">
+      <c r="B73" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C73" s="10" t="s">
@@ -3261,7 +3261,7 @@
         <v>48</v>
       </c>
       <c r="I73" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J73" s="25">
         <v>1</v>
@@ -3272,7 +3272,7 @@
       <c r="A74" s="23">
         <v>72</v>
       </c>
-      <c r="B74" s="37"/>
+      <c r="B74" s="63"/>
       <c r="C74" s="13"/>
       <c r="D74" s="9" t="s">
         <v>46</v>
@@ -3285,8 +3285,8 @@
       <c r="H74" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I74" s="40" t="s">
-        <v>196</v>
+      <c r="I74" s="64" t="s">
+        <v>195</v>
       </c>
       <c r="J74" s="25">
         <v>1</v>
@@ -3297,7 +3297,7 @@
       <c r="A75" s="23">
         <v>73</v>
       </c>
-      <c r="B75" s="37"/>
+      <c r="B75" s="63"/>
       <c r="C75" s="13"/>
       <c r="D75" s="9" t="s">
         <v>47</v>
@@ -3310,7 +3310,7 @@
       <c r="H75" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I75" s="40"/>
+      <c r="I75" s="64"/>
       <c r="J75" s="25">
         <v>1</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="A76" s="23">
         <v>74</v>
       </c>
-      <c r="B76" s="37"/>
+      <c r="B76" s="63"/>
       <c r="C76" s="16"/>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
@@ -3333,7 +3333,7 @@
       <c r="H76" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I76" s="40"/>
+      <c r="I76" s="64"/>
       <c r="J76" s="25">
         <v>1</v>
       </c>
@@ -3343,7 +3343,7 @@
       <c r="A77" s="23">
         <v>75</v>
       </c>
-      <c r="B77" s="37"/>
+      <c r="B77" s="63"/>
       <c r="C77" s="16"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
@@ -3356,7 +3356,7 @@
       <c r="H77" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I77" s="40"/>
+      <c r="I77" s="64"/>
       <c r="J77" s="25">
         <v>1</v>
       </c>
@@ -3366,7 +3366,7 @@
       <c r="A78" s="23">
         <v>76</v>
       </c>
-      <c r="B78" s="37"/>
+      <c r="B78" s="63"/>
       <c r="C78" s="13"/>
       <c r="D78" s="9" t="s">
         <v>42</v>
@@ -3377,9 +3377,9 @@
         <v>41</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="I78" s="40"/>
+        <v>168</v>
+      </c>
+      <c r="I78" s="64"/>
       <c r="J78" s="24">
         <v>2</v>
       </c>
@@ -3389,27 +3389,27 @@
       <c r="A79" s="23">
         <v>77</v>
       </c>
-      <c r="B79" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="C79" s="48"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
-      <c r="F79" s="48"/>
-      <c r="G79" s="48"/>
-      <c r="H79" s="48"/>
-      <c r="I79" s="48"/>
-      <c r="J79" s="48"/>
+      <c r="B79" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="39"/>
+      <c r="I79" s="39"/>
+      <c r="J79" s="39"/>
     </row>
     <row r="80" spans="1:12" ht="16.5" customHeight="1">
       <c r="A80" s="23">
         <v>78</v>
       </c>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="40" t="s">
         <v>88</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
@@ -3418,7 +3418,7 @@
         <v>12</v>
       </c>
       <c r="H80" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I80" s="28"/>
       <c r="J80" s="25">
@@ -3431,16 +3431,16 @@
       <c r="A81" s="23">
         <v>79</v>
       </c>
-      <c r="B81" s="41"/>
+      <c r="B81" s="40"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I81" s="29"/>
       <c r="J81" s="25">
@@ -3453,19 +3453,19 @@
       <c r="A82" s="23">
         <v>80</v>
       </c>
-      <c r="B82" s="41"/>
+      <c r="B82" s="40"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
       <c r="H82" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I82" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J82" s="25">
         <v>2</v>
@@ -3477,9 +3477,9 @@
       <c r="A83" s="23">
         <v>81</v>
       </c>
-      <c r="B83" s="41"/>
+      <c r="B83" s="40"/>
       <c r="C83" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
@@ -3488,7 +3488,7 @@
         <v>84</v>
       </c>
       <c r="H83" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I83" s="28"/>
       <c r="J83" s="25">
@@ -3501,7 +3501,7 @@
       <c r="A84" s="23">
         <v>82</v>
       </c>
-      <c r="B84" s="41"/>
+      <c r="B84" s="40"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9" t="s">
         <v>79</v>
@@ -3510,7 +3510,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I84" s="29"/>
       <c r="J84" s="25">
@@ -3523,18 +3523,18 @@
       <c r="A85" s="23">
         <v>83</v>
       </c>
-      <c r="B85" s="41"/>
+      <c r="B85" s="40"/>
       <c r="C85" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H85" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I85" s="28"/>
       <c r="J85" s="25">
@@ -3547,16 +3547,16 @@
       <c r="A86" s="23">
         <v>84</v>
       </c>
-      <c r="B86" s="41"/>
+      <c r="B86" s="40"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
       <c r="H86" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I86" s="29"/>
       <c r="J86" s="25">
@@ -3569,18 +3569,18 @@
       <c r="A87" s="23">
         <v>85</v>
       </c>
-      <c r="B87" s="41"/>
+      <c r="B87" s="40"/>
       <c r="C87" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H87" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I87" s="28"/>
       <c r="J87" s="25">
@@ -3783,6 +3783,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="B61:J61"/>
+    <mergeCell ref="I74:I78"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="B72:J72"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B11:B14"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B79:J79"/>
     <mergeCell ref="B80:B87"/>
@@ -3799,18 +3811,6 @@
     <mergeCell ref="B48:B52"/>
     <mergeCell ref="B53:J53"/>
     <mergeCell ref="I54:I56"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="B61:J61"/>
-    <mergeCell ref="I74:I78"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="B72:J72"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>